<commit_message>
10-OCT-2024 One question solved on binary tree
</commit_message>
<xml_diff>
--- a/Detail_About_Problems_I_Solved/Book1.xlsx
+++ b/Detail_About_Problems_I_Solved/Book1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="107">
   <si>
     <t xml:space="preserve"> Date </t>
   </si>
@@ -345,6 +345,24 @@
   </si>
   <si>
     <t>Stack +without stack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                    Binary Tree</t>
+  </si>
+  <si>
+    <t>Subtree of another tree</t>
+  </si>
+  <si>
+    <t>Recursion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculate max depth of binary tree </t>
+  </si>
+  <si>
+    <t>I have solved it in first attempt</t>
+  </si>
+  <si>
+    <t>15/10/2024</t>
   </si>
 </sst>
 </file>
@@ -732,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,6 +1354,36 @@
       </c>
       <c r="G67" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B68" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
+        <v>45580</v>
+      </c>
+      <c r="B69" t="s">
+        <v>102</v>
+      </c>
+      <c r="C69" t="s">
+        <v>103</v>
+      </c>
+      <c r="G69" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B70" t="s">
+        <v>104</v>
+      </c>
+      <c r="H70" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
16-OCT-2024 Two question solved on binary tree
</commit_message>
<xml_diff>
--- a/Detail_About_Problems_I_Solved/Book1.xlsx
+++ b/Detail_About_Problems_I_Solved/Book1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="109">
   <si>
     <t xml:space="preserve"> Date </t>
   </si>
@@ -363,6 +363,12 @@
   </si>
   <si>
     <t>15/10/2024</t>
+  </si>
+  <si>
+    <t>Invert binary tree</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -438,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -449,6 +455,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="C53" workbookViewId="0">
+      <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,6 +1391,20 @@
       </c>
       <c r="H70" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="8">
+        <v>45581</v>
+      </c>
+      <c r="B71" t="s">
+        <v>107</v>
+      </c>
+      <c r="G71" t="s">
+        <v>87</v>
+      </c>
+      <c r="H71" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dfs and bfs added in UsingAdjacencyList.java in Graphs Folder in date(11/19/2024)
</commit_message>
<xml_diff>
--- a/Detail_About_Problems_I_Solved/Book1.xlsx
+++ b/Detail_About_Problems_I_Solved/Book1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="110">
   <si>
     <t xml:space="preserve"> Date </t>
   </si>
@@ -353,9 +353,6 @@
     <t>Subtree of another tree</t>
   </si>
   <si>
-    <t>Recursion</t>
-  </si>
-  <si>
     <t xml:space="preserve">calculate max depth of binary tree </t>
   </si>
   <si>
@@ -369,6 +366,12 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  10/23/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isSame </t>
   </si>
 </sst>
 </file>
@@ -757,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C53" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+      <selection activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,7 +1379,7 @@
         <v>102</v>
       </c>
       <c r="C69" t="s">
-        <v>103</v>
+        <v>10</v>
       </c>
       <c r="G69" t="s">
         <v>87</v>
@@ -1384,13 +1387,13 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B70" t="s">
+        <v>103</v>
+      </c>
+      <c r="H70" t="s">
         <v>104</v>
-      </c>
-      <c r="H70" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -1398,13 +1401,30 @@
         <v>45581</v>
       </c>
       <c r="B71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G71" t="s">
         <v>87</v>
       </c>
       <c r="H71" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>108</v>
+      </c>
+      <c r="B73" t="s">
+        <v>109</v>
+      </c>
+      <c r="C73" t="s">
+        <v>10</v>
+      </c>
+      <c r="G73" t="s">
+        <v>87</v>
+      </c>
+      <c r="H73" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
graph updated - dijkstra added as well
</commit_message>
<xml_diff>
--- a/Detail_About_Problems_I_Solved/Book1.xlsx
+++ b/Detail_About_Problems_I_Solved/Book1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="117">
   <si>
     <t xml:space="preserve"> Date </t>
   </si>
@@ -373,12 +373,33 @@
   <si>
     <t xml:space="preserve">isSame </t>
   </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>All Paths From Source to Target</t>
+  </si>
+  <si>
+    <t>leatcide</t>
+  </si>
+  <si>
+    <t>DFS</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Rotting Oranges</t>
+  </si>
+  <si>
+    <t>BFS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -426,6 +447,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -444,10 +488,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -459,8 +504,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -760,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C53" workbookViewId="0">
-      <selection activeCell="J68" sqref="J68"/>
+    <sheetView tabSelected="1" topLeftCell="C64" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,6 +1474,45 @@
       </c>
       <c r="H73" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B76" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="G76" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="8">
+        <v>45623</v>
+      </c>
+      <c r="B77" t="s">
+        <v>111</v>
+      </c>
+      <c r="C77" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D77" t="s">
+        <v>113</v>
+      </c>
+      <c r="H77" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="8">
+        <v>45626</v>
+      </c>
+      <c r="B79" t="s">
+        <v>115</v>
+      </c>
+      <c r="C79" t="s">
+        <v>10</v>
+      </c>
+      <c r="D79" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>